<commit_message>
Added links to meetup page.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox/School/Teaching/EPSY630 2021 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A12A6A-CEC2-0547-AE50-E54DC7DF3B9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629423EF-F179-7541-835D-1FF8CC023074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="12400" windowWidth="27440" windowHeight="15200" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>TBD</t>
+  </si>
+  <si>
+    <t>[Video](https://youtu.be/kxa3gb7kSCU), [Slides](/slides/00-Intro_to_Course.html)</t>
   </si>
 </sst>
 </file>
@@ -719,7 +722,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -751,6 +754,9 @@
       </c>
       <c r="C2" t="s">
         <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added assignments and slides.
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox/School/Teaching/EPSY630 2021 Spring/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629423EF-F179-7541-835D-1FF8CC023074}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0958E64-1F57-124F-B039-A2E0088B3D29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1680" yWindow="12400" windowWidth="27440" windowHeight="15200" activeTab="1" xr2:uid="{A772458D-4E7B-8249-8B6B-34FE7D5BD316}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="27">
   <si>
     <t>Date</t>
   </si>
@@ -105,6 +105,9 @@
   </si>
   <si>
     <t>[Video](https://youtu.be/kxa3gb7kSCU), [Slides](/slides/00-Intro_to_Course.html)</t>
+  </si>
+  <si>
+    <t>[Video](https://youtu.be/RNUJKKj3kL4), [Slides](/slides/2021-02-09-Intro_to_R.html)</t>
   </si>
 </sst>
 </file>
@@ -722,7 +725,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,6 +771,9 @@
       </c>
       <c r="C3" t="s">
         <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>